<commit_message>
add updatePrice.py fou updating price only
</commit_message>
<xml_diff>
--- a/Testfiles/output.xlsx
+++ b/Testfiles/output.xlsx
@@ -599,7 +599,7 @@
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>Depth: 12, Height: 30, Width: 09</t>
+          <t>Width:09, Height:30, Depth:12</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
@@ -2834,7 +2834,7 @@
       </c>
       <c r="R42" t="inlineStr">
         <is>
-          <t>Depth: 12, Height: 30, Width: 12</t>
+          <t>Width:12, Height:30, Depth:12</t>
         </is>
       </c>
       <c r="S42" t="inlineStr">
@@ -5069,7 +5069,7 @@
       </c>
       <c r="R82" t="inlineStr">
         <is>
-          <t>Depth: 12, Height: 30, Width: 15</t>
+          <t>Width:15, Height:30, Depth:12</t>
         </is>
       </c>
       <c r="S82" t="inlineStr">
@@ -7304,7 +7304,7 @@
       </c>
       <c r="R122" t="inlineStr">
         <is>
-          <t>Depth: 12, Height: 30, Width: 18</t>
+          <t>Width:18, Height:30, Depth:12</t>
         </is>
       </c>
       <c r="S122" t="inlineStr">
@@ -9539,7 +9539,7 @@
       </c>
       <c r="R162" t="inlineStr">
         <is>
-          <t>Depth: 12, Height: 30, Width: 21</t>
+          <t>Width:21, Height:30, Depth:12</t>
         </is>
       </c>
       <c r="S162" t="inlineStr">
@@ -11774,7 +11774,7 @@
       </c>
       <c r="R202" t="inlineStr">
         <is>
-          <t>Depth: 12, Height: 30, Width: 24</t>
+          <t>Width:24, Height:30, Depth:12</t>
         </is>
       </c>
       <c r="S202" t="inlineStr">
@@ -14009,7 +14009,7 @@
       </c>
       <c r="R242" t="inlineStr">
         <is>
-          <t>Depth: 24, Height: 30, Width: 24</t>
+          <t>Width:24, Height:30, Depth:24</t>
         </is>
       </c>
       <c r="S242" t="inlineStr">
@@ -16244,7 +16244,7 @@
       </c>
       <c r="R282" t="inlineStr">
         <is>
-          <t>Depth: 24, Height: 36, Width: 24</t>
+          <t>Width:24, Height:36, Depth:24</t>
         </is>
       </c>
       <c r="S282" t="inlineStr">
@@ -18479,7 +18479,7 @@
       </c>
       <c r="R322" t="inlineStr">
         <is>
-          <t>Depth: 24, Height: 39, Width: 24</t>
+          <t>Width:24, Height:39, Depth:24</t>
         </is>
       </c>
       <c r="S322" t="inlineStr">
@@ -20714,7 +20714,7 @@
       </c>
       <c r="R362" t="inlineStr">
         <is>
-          <t>Depth: 24, Height: 42, Width: 24</t>
+          <t>Width:24, Height:42, Depth:24</t>
         </is>
       </c>
       <c r="S362" t="inlineStr">
@@ -22949,7 +22949,7 @@
       </c>
       <c r="R402" t="inlineStr">
         <is>
-          <t>Depth: 24, Height: 30, Width: 24</t>
+          <t>Width:24, Height:30, Depth:24</t>
         </is>
       </c>
       <c r="S402" t="inlineStr">
@@ -25184,7 +25184,7 @@
       </c>
       <c r="R442" t="inlineStr">
         <is>
-          <t>Depth: 24, Height: 36, Width: 24</t>
+          <t>Width:24, Height:36, Depth:24</t>
         </is>
       </c>
       <c r="S442" t="inlineStr">
@@ -27404,7 +27404,7 @@
       </c>
       <c r="O482" t="inlineStr">
         <is>
-          <t>base_cabinet_1ro, 33W, 34.5H, 24D</t>
+          <t>base_cabinet_1ro, 33W, 34.5H, 24D, base_cabinet</t>
         </is>
       </c>
       <c r="P482" t="inlineStr">
@@ -27419,7 +27419,7 @@
       </c>
       <c r="R482" t="inlineStr">
         <is>
-          <t>Depth: 24, Height: 34.5, Width: 33</t>
+          <t>Width:33, Height:34.5, Depth:24</t>
         </is>
       </c>
       <c r="S482" t="inlineStr">
@@ -29639,7 +29639,7 @@
       </c>
       <c r="O522" t="inlineStr">
         <is>
-          <t>base_cabinet_1ro, 36W, 34.5H, 24D</t>
+          <t>base_cabinet_1ro, 36W, 34.5H, 24D, base_cabinet</t>
         </is>
       </c>
       <c r="P522" t="inlineStr">
@@ -29654,7 +29654,7 @@
       </c>
       <c r="R522" t="inlineStr">
         <is>
-          <t>Depth: 24, Height: 34.5, Width: 36</t>
+          <t>Width:36, Height:34.5, Depth:24</t>
         </is>
       </c>
       <c r="S522" t="inlineStr">
@@ -31874,7 +31874,7 @@
       </c>
       <c r="O562" t="inlineStr">
         <is>
-          <t>base_cabinet_2ro, 12W, 34.5H, 24D</t>
+          <t>base_cabinet_2ro, 12W, 34.5H, 24D, base_cabinet</t>
         </is>
       </c>
       <c r="P562" t="inlineStr">
@@ -31889,7 +31889,7 @@
       </c>
       <c r="R562" t="inlineStr">
         <is>
-          <t>Depth: 24, Height: 34.5, Width: 12</t>
+          <t>Width:12, Height:34.5, Depth:24</t>
         </is>
       </c>
       <c r="S562" t="inlineStr">
@@ -34124,7 +34124,7 @@
       </c>
       <c r="R602" t="inlineStr">
         <is>
-          <t>Depth: 24, Height: 34.5, Width: 24</t>
+          <t>Width:24, Height:34.5, Depth:24</t>
         </is>
       </c>
       <c r="S602" t="inlineStr">
@@ -36359,7 +36359,7 @@
       </c>
       <c r="R642" t="inlineStr">
         <is>
-          <t>Depth: 24, Height: 34.5, Width: 27</t>
+          <t>Width:27, Height:34.5, Depth:24</t>
         </is>
       </c>
       <c r="S642" t="inlineStr">
@@ -38594,7 +38594,7 @@
       </c>
       <c r="R682" t="inlineStr">
         <is>
-          <t>Depth: 24, Height: 34.5, Width: 39</t>
+          <t>Width:39, Height:34.5, Depth:24</t>
         </is>
       </c>
       <c r="S682" t="inlineStr">
@@ -40829,7 +40829,7 @@
       </c>
       <c r="R722" t="inlineStr">
         <is>
-          <t>Depth: 24, Height: 34.5, Width: 30</t>
+          <t>Width:30, Height:34.5, Depth:24</t>
         </is>
       </c>
       <c r="S722" t="inlineStr">
@@ -43064,7 +43064,7 @@
       </c>
       <c r="R762" t="inlineStr">
         <is>
-          <t>Depth: 24, Height: 84, Width: 30</t>
+          <t>Width:30, Height:84, Depth:24</t>
         </is>
       </c>
       <c r="S762" t="inlineStr">

</xml_diff>